<commit_message>
Guardando cambios en el excel
</commit_message>
<xml_diff>
--- a/Agenda.xlsx
+++ b/Agenda.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Dropbox\MisionTIC\Ciclo_4\RadioSun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Dropbox\MisionTIC\Ciclo_4\RadioSunV19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EEB8367-72A6-48A1-8642-7095F7D7BB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A335B4D-468B-4DF7-8AF9-158C4EAF0EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C90EBDA1-DE55-4DDA-9C84-277746755D5D}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>LOGIN</t>
   </si>
@@ -80,6 +80,21 @@
   </si>
   <si>
     <t>Mostrará toda la información de cuantos paneles necesita el sistema.</t>
+  </si>
+  <si>
+    <t>Jorge</t>
+  </si>
+  <si>
+    <t>Juan Carlos</t>
+  </si>
+  <si>
+    <t>Freire</t>
+  </si>
+  <si>
+    <t>Jair</t>
+  </si>
+  <si>
+    <t>ENCARGADO</t>
   </si>
 </sst>
 </file>
@@ -480,82 +495,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9299635-DA0D-4629-A5D9-236002CA130D}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="C8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>